<commit_message>
added new html results d3 graph page version updated to 0.0.16
</commit_message>
<xml_diff>
--- a/exampleProblems/eserine/Eserine.xlsx
+++ b/exampleProblems/eserine/Eserine.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/vsmw51_durham_ac_uk/Documents/projects/programming/2022/python/python/rdkit37/projects/simpleNMR/exampleProblems/eserine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{52AA9AB8-45BF-FB4B-B1EC-A72F7C6339C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC97E1AC-4578-4FA7-9A24-44248A745E9F}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{52AA9AB8-45BF-FB4B-B1EC-A72F7C6339C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAACAC4D-DA89-5040-A553-BF6A31194A6B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="molecule" sheetId="9" r:id="rId1"/>
-    <sheet name="H1_1D" sheetId="1" r:id="rId2"/>
-    <sheet name="HSQC" sheetId="4" r:id="rId3"/>
-    <sheet name="COSY" sheetId="5" r:id="rId4"/>
-    <sheet name="HMBC" sheetId="8" r:id="rId5"/>
-    <sheet name="C13_1D" sheetId="2" r:id="rId6"/>
+    <sheet name="HSQC" sheetId="4" r:id="rId2"/>
+    <sheet name="COSY" sheetId="12" r:id="rId3"/>
+    <sheet name="HMBC" sheetId="8" r:id="rId4"/>
+    <sheet name="C13_1D" sheetId="2" r:id="rId5"/>
+    <sheet name="H1_1D" sheetId="11" r:id="rId6"/>
     <sheet name="H1_pureshift" sheetId="3" r:id="rId7"/>
     <sheet name="NOESY" sheetId="10" r:id="rId8"/>
   </sheets>
@@ -661,7 +661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -689,390 +689,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col min="8" max="8" width="32.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="17">
-      <c r="A1" s="10"/>
-      <c r="B1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="17">
-      <c r="A2" s="10">
-        <v>1</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="10">
-        <v>6.3179999999999996</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="10">
-        <v>1</v>
-      </c>
-      <c r="F2" s="10">
-        <v>1</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="10">
-        <v>8.3699999999999992</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="17">
-      <c r="A3" s="10">
-        <v>2</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="10">
-        <v>6.7439999999999998</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="10">
-        <v>1</v>
-      </c>
-      <c r="F3" s="10">
-        <v>0.97</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="10">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="17">
-      <c r="A4" s="10">
-        <v>3</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="10">
-        <v>6.7830000000000004</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="10">
-        <v>1</v>
-      </c>
-      <c r="F4" s="10">
-        <v>0.98</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="17">
-      <c r="A5" s="10">
-        <v>4</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="10">
-        <v>5.04</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="10">
-        <v>1</v>
-      </c>
-      <c r="F5" s="10">
-        <v>0.86</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="17">
-      <c r="A6" s="10">
-        <v>5</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="10">
-        <v>4.09</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="10">
-        <v>1</v>
-      </c>
-      <c r="F6" s="10">
-        <v>0.98</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="17">
-      <c r="A7" s="10">
-        <v>6</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="10">
-        <v>2.9009999999999998</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="10">
-        <v>3</v>
-      </c>
-      <c r="F7" s="10">
-        <v>3.22</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="17">
-      <c r="A8" s="10">
-        <v>7</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="10">
-        <v>2.8380000000000001</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="10">
-        <v>3</v>
-      </c>
-      <c r="F8" s="10">
-        <v>2.65</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="10">
-        <v>4.92</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="17">
-      <c r="A9" s="10">
-        <v>8</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="10">
-        <v>2.7</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="10">
-        <v>1</v>
-      </c>
-      <c r="F9" s="10">
-        <v>1.03</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="17">
-      <c r="A10" s="10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="10">
-        <v>2.6320000000000001</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="10">
-        <v>1</v>
-      </c>
-      <c r="F10" s="10">
-        <v>1.04</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="17">
-      <c r="A11" s="10">
-        <v>10</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="10">
-        <v>2.5379999999999998</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="10">
-        <v>3</v>
-      </c>
-      <c r="F11" s="10">
-        <v>2.99</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="17">
-      <c r="A12" s="10">
-        <v>11</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="10">
-        <v>1.9259999999999999</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="10">
-        <v>2</v>
-      </c>
-      <c r="F12" s="10">
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="17">
-      <c r="A13" s="10">
-        <v>12</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="10">
-        <v>1.409</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="10">
-        <v>3</v>
-      </c>
-      <c r="F13" s="10">
-        <v>2.97</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
@@ -1480,17 +1096,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:V35"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03920CC0-8921-7F4A-B4E0-085795C1CB49}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:22" ht="17">
+    <row r="1" spans="1:11" ht="17">
       <c r="A1" s="11"/>
       <c r="B1" s="11" t="s">
         <v>20</v>
@@ -1522,19 +1138,8 @@
       <c r="K1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="4"/>
-    </row>
-    <row r="2" spans="1:22" ht="17">
+    </row>
+    <row r="2" spans="1:11" ht="17">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -1564,10 +1169,8 @@
       </c>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="6"/>
-    </row>
-    <row r="3" spans="1:22" ht="17">
+    </row>
+    <row r="3" spans="1:11" ht="17">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -1597,10 +1200,8 @@
       </c>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="6"/>
-    </row>
-    <row r="4" spans="1:22" ht="17">
+    </row>
+    <row r="4" spans="1:11" ht="17">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -1630,422 +1231,13 @@
       </c>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="6"/>
-    </row>
-    <row r="5" spans="1:22">
-      <c r="A5" s="5"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="6"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="6"/>
-    </row>
-    <row r="6" spans="1:22">
-      <c r="A6" s="5"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="6"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="6"/>
-    </row>
-    <row r="7" spans="1:22">
-      <c r="A7" s="5"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="6"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="6"/>
-    </row>
-    <row r="8" spans="1:22">
-      <c r="A8" s="5"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="6"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="6"/>
-    </row>
-    <row r="9" spans="1:22">
-      <c r="A9" s="5"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="6"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="6"/>
-    </row>
-    <row r="10" spans="1:22">
-      <c r="A10" s="5"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="6"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="6"/>
-    </row>
-    <row r="11" spans="1:22">
-      <c r="A11" s="5"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="6"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="6"/>
-    </row>
-    <row r="12" spans="1:22">
-      <c r="A12" s="5"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="6"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="6"/>
-    </row>
-    <row r="13" spans="1:22">
-      <c r="A13" s="5"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="6"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="6"/>
-    </row>
-    <row r="14" spans="1:22">
-      <c r="A14" s="5"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="6"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="6"/>
-    </row>
-    <row r="15" spans="1:22">
-      <c r="A15" s="5"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="6"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="6"/>
-    </row>
-    <row r="16" spans="1:22">
-      <c r="A16" s="5"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="6"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="6"/>
-    </row>
-    <row r="17" spans="1:22">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="9"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="9"/>
-    </row>
-    <row r="18" spans="1:22">
-      <c r="A18" s="5"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="9"/>
-    </row>
-    <row r="19" spans="1:22">
-      <c r="A19" s="5"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:22">
-      <c r="A20" s="5"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:22">
-      <c r="A21" s="5"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:22">
-      <c r="A22" s="5"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:22">
-      <c r="A23" s="5"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:22">
-      <c r="A24" s="5"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:22">
-      <c r="A25" s="5"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:22">
-      <c r="A26" s="5"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:22">
-      <c r="A27" s="5"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:22">
-      <c r="A28" s="5"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:22">
-      <c r="A29" s="5"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:22">
-      <c r="A30" s="5"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:22">
-      <c r="A31" s="5"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:22">
-      <c r="A32" s="5"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="5"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="7"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:V31"/>
   <sheetViews>
@@ -2858,7 +2050,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
@@ -3273,6 +2465,386 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C109330D-3DC1-4442-8B5B-19F759A9C0D6}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="17">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="10">
+        <v>6.3179999999999996</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="10">
+        <v>1</v>
+      </c>
+      <c r="F2" s="10">
+        <v>1</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="10">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="10">
+        <v>6.7439999999999998</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="10">
+        <v>1</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0.97</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="10">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="10">
+        <v>6.7830000000000004</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="10">
+        <v>1</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0.98</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="10">
+        <v>5.04</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.86</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="10">
+        <v>4.09</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="10">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.98</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="10">
+        <v>2.9009999999999998</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="10">
+        <v>3</v>
+      </c>
+      <c r="F7" s="10">
+        <v>3.22</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="10">
+        <v>2.8380000000000001</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="10">
+        <v>3</v>
+      </c>
+      <c r="F8" s="10">
+        <v>2.65</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="10">
+        <v>4.92</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="10">
+        <v>2.7</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="10">
+        <v>1</v>
+      </c>
+      <c r="F9" s="10">
+        <v>1.03</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="10">
+        <v>2.6320000000000001</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="10">
+        <v>1.04</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="10">
+        <v>2.5379999999999998</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="10">
+        <v>3</v>
+      </c>
+      <c r="F11" s="10">
+        <v>2.99</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="17">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="10">
+        <v>1.9259999999999999</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="10">
+        <v>2</v>
+      </c>
+      <c r="F12" s="10">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="17">
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="10">
+        <v>1.409</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="10">
+        <v>3</v>
+      </c>
+      <c r="F13" s="10">
+        <v>2.97</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3477,21 +3049,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100155B07917A39914F9664B9093559A33D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fbeff89c08116489e82681c46e7ae15d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f6191221-55a2-427d-afce-6bfcc029a585" xmlns:ns4="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a905948312a67a3512ded1d64743b24d" ns3:_="" ns4:_="">
     <xsd:import namespace="f6191221-55a2-427d-afce-6bfcc029a585"/>
@@ -3708,32 +3265,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44668820-0664-4E62-A660-376AF03334EF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f"/>
-    <ds:schemaRef ds:uri="f6191221-55a2-427d-afce-6bfcc029a585"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCEF473A-5319-4ED2-888F-44217AC86176}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3750,4 +3297,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44668820-0664-4E62-A660-376AF03334EF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="f6191221-55a2-427d-afce-6bfcc029a585"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>